<commit_message>
[IMP] account: unify reconciliation of import
Purpose
-------

Allow to reconcile entries during import easily.
* Have one uniform way of doing it
  - fix bugs only once
  - reduce number of fields
  - make it generic and not only for some imports
* avoid the need to post during imports
  - faster to import, can import bigger batches, because we do neither
    post or reconcile, both are among the most time consuming steps.
  - still allows to check the data before posting if needed
* make splitting import into smaller batches easier because the
  reconciliation is not cut/dependent on the batches anymore
* allow to reconcile entries in the future by using the same mechanism
  (i.e. cut-off)

Implementation
--------------

Allow setting the matching number to `I*` manually, where `*` can be
anything. When posting the last item with the same manually set number,
we will reconcile all the lines with the same number.

task-3593885
</commit_message>
<xml_diff>
--- a/addons/account/static/xls/aml_import_template.xlsx
+++ b/addons/account/static/xls/aml_import_template.xlsx
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
   <si>
     <t xml:space="preserve">journal_id</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t xml:space="preserve">credit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">matching_number</t>
   </si>
   <si>
     <t xml:space="preserve">MISC</t>
@@ -120,7 +123,16 @@
     <t xml:space="preserve">Salary November 2021</t>
   </si>
   <si>
-    <t xml:space="preserve">       </t>
+    <t xml:space="preserve">R1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BNK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BNK/2021/00001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payment Salary November 2021</t>
   </si>
   <si>
     <t xml:space="preserve">(Optional) Import Journal Items</t>
@@ -592,10 +604,10 @@
   <dimension ref="A1:V1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.87"/>
@@ -607,7 +619,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.63"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -632,7 +644,9 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3"/>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -649,19 +663,19 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="5" t="n">
         <v>44536</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>700200</v>
@@ -687,19 +701,19 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="5" t="n">
         <v>44536</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="6" t="n">
         <v>700200</v>
@@ -725,19 +739,19 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="5" t="n">
         <v>44536</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4" s="6" t="n">
         <v>400000</v>
@@ -761,19 +775,19 @@
       <c r="U4" s="3"/>
       <c r="V4" s="3"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="9" t="n">
         <v>44531</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F5" s="6" t="n">
         <v>455000</v>
@@ -782,7 +796,9 @@
       <c r="H5" s="7" t="n">
         <v>11750</v>
       </c>
-      <c r="I5" s="3"/>
+      <c r="I5" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
@@ -797,19 +813,19 @@
       <c r="U5" s="3"/>
       <c r="V5" s="3"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" s="9" t="n">
         <v>44531</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F6" s="6" t="n">
         <v>620200</v>
@@ -833,18 +849,30 @@
       <c r="U6" s="3"/>
       <c r="V6" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3"/>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="B7" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="3"/>
+      <c r="C7" s="9" t="n">
+        <v>44545</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="6" t="n">
+        <v>455000</v>
+      </c>
+      <c r="G7" s="10" t="n">
+        <v>11750</v>
+      </c>
+      <c r="H7" s="7"/>
+      <c r="I7" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
@@ -859,15 +887,27 @@
       <c r="U7" s="3"/>
       <c r="V7" s="3"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="9" t="n">
+        <v>44545</v>
+      </c>
       <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
+      <c r="E8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="6" t="n">
+        <v>550003</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="10" t="n">
+        <v>11750</v>
+      </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -17559,15 +17599,15 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="120.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="120.77"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -17596,7 +17636,7 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="3"/>
@@ -17652,10 +17692,10 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -17683,10 +17723,10 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -17714,10 +17754,10 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="17" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -17745,10 +17785,10 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="19" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -17776,7 +17816,7 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="19" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -17808,7 +17848,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -17839,7 +17879,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -17867,10 +17907,10 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="19" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>

</xml_diff>